<commit_message>
xlsx: update till p27.cpp
</commit_message>
<xml_diff>
--- a/exercises/cpp-concurrency-in-action/cpp-concurrency-in-action-progress-summary.xlsx
+++ b/exercises/cpp-concurrency-in-action/cpp-concurrency-in-action-progress-summary.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\git\codelab\codelab-cpp\exercises\cpp-concurrency-in-action\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6DF98020-9786-40A2-966D-E55005731F7A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{102F9874-BB7F-4F4C-8549-E8C39404B0CE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{493514F6-972A-4E7F-BD62-E5E01A93C8DE}"/>
   </bookViews>
@@ -33,8 +33,63 @@
 </workbook>
 </file>
 
+<file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+  <authors>
+    <author>Guyen G</author>
+  </authors>
+  <commentList>
+    <comment ref="E14" authorId="0" shapeId="0" xr:uid="{24E8444F-B76D-4EC3-98A9-12F5924B7705}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Guyen G:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
++ for i in $1
++ sudo g++ p27.cpp -o p27.out
+p27.cpp: In constructor ‘scoped_thread::scoped_thread(std::thread)’:
+p27.cpp:15:57: error: cannot bind non-const lvalue reference of type ‘std::thread&amp;’ to an rvalue of type ‘std::remove_reference&lt;std::thread&amp;&gt;::type’ {aka ‘std::thread’}
+   15 |     explicit scoped_thread(std::thread t_) : t(std::move(t_)) {
+      |                                                ~~~~~~~~~^~~~
+p27.cpp: In function ‘void f()’:
+p27.cpp:57:20: warning: parentheses were disambiguated as a function declaration [-Wvexing-parse]
+   57 |     scoped_thread t(std::thread(func(some_local_state)));
+      |                    ^~~~~~~~~~~~~~~~~~~~~~~~~~~~~~~~~~~~~
+p27.cpp:57:20: note: replace parentheses with braces to declare a variable
+   57 |     scoped_thread t(std::thread(func(some_local_state)));
+      |                    ^~~~~~~~~~~~~~~~~~~~~~~~~~~~~~~~~~~~~
+      |                    -
+      |                    {                                   -
+      |                                                        }
++ [[ 1 -eq 0 ]]
++ exit 1
+++ ./p27.out
+./run.sh: line 6: ./p27.out: No such file or directory
+[guyen@localhost ch2]$
+</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="35">
   <si>
     <t>ch2</t>
   </si>
@@ -120,12 +175,37 @@
   <si>
     <t>The only question is why compile error when std::move is not used: //std::thread t(process_big_object, p); &lt;-- tried to see if cout after t.join() will printer same address but huge compiler error.</t>
   </si>
+  <si>
+    <t>p19.cpp</t>
+  </si>
+  <si>
+    <t>Throw exception but it is not seeming to catch exception. The sample code helper/exception.c seems to be catching ok, not sure what the difference is.
+Next update: seems to be working as of 191a2ccd8d87dbf5986c1c6b48f0a71351ea9b30</t>
+  </si>
+  <si>
+    <t>OK</t>
+  </si>
+  <si>
+    <t>p20.cpp</t>
+  </si>
+  <si>
+    <t>ok</t>
+  </si>
+  <si>
+    <t>p27.cpp</t>
+  </si>
+  <si>
+    <t>not working</t>
+  </si>
+  <si>
+    <t>see note</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -156,6 +236,19 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="4">
@@ -206,7 +299,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -221,9 +314,6 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
@@ -540,11 +630,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5B62B63B-69FD-414D-A654-5AB40C224B5D}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5B62B63B-69FD-414D-A654-5AB40C224B5D}">
   <dimension ref="A1:E581"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+    <sheetView tabSelected="1" topLeftCell="C7" workbookViewId="0">
+      <selection activeCell="E15" sqref="E15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="30.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -665,7 +755,7 @@
       <c r="B9" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="C9" s="6" t="s">
+      <c r="C9" s="2" t="s">
         <v>21</v>
       </c>
       <c r="D9" s="2"/>
@@ -697,26 +787,42 @@
         <v>26</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:5" ht="72" x14ac:dyDescent="0.3">
       <c r="A12" s="2"/>
-      <c r="B12" s="2"/>
+      <c r="B12" s="2" t="s">
+        <v>27</v>
+      </c>
       <c r="C12" s="2"/>
-      <c r="D12" s="2"/>
-      <c r="E12" s="2"/>
+      <c r="D12" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="E12" s="2" t="s">
+        <v>28</v>
+      </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A13" s="2"/>
-      <c r="B13" s="2"/>
+      <c r="B13" s="2" t="s">
+        <v>30</v>
+      </c>
       <c r="C13" s="2"/>
-      <c r="D13" s="2"/>
+      <c r="D13" s="2" t="s">
+        <v>31</v>
+      </c>
       <c r="E13" s="2"/>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A14" s="2"/>
-      <c r="B14" s="2"/>
+      <c r="B14" s="2" t="s">
+        <v>32</v>
+      </c>
       <c r="C14" s="2"/>
-      <c r="D14" s="2"/>
-      <c r="E14" s="2"/>
+      <c r="D14" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="E14" s="2" t="s">
+        <v>34</v>
+      </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A15" s="2"/>
@@ -4693,5 +4799,6 @@
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId2"/>
+  <legacyDrawing r:id="rId3"/>
 </worksheet>
 </file>
</xml_diff>